<commit_message>
Agrego:   - Test para ver si funciona el lector de archivos de excel   - Organizacion y miembro relacion
</commit_message>
<xml_diff>
--- a/src/main/resources/ejemploDA.xlsx
+++ b/src/main/resources/ejemploDA.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Actividad</t>
   </si>
@@ -37,31 +37,64 @@
     <t>Gas Natural</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>Mensual</t>
   </si>
   <si>
-    <t>Diese/Gasoil</t>
+    <t>12/2012</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>Anual</t>
   </si>
   <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>Gasoil</t>
+  </si>
+  <si>
     <t>Kerosene</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>Fuel Oil</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>Nafta</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>Carbon</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>Carbon de leña</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>Lena</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>Combustión móvil</t>
@@ -92,10 +125,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/yyyy"/>
-  </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -107,13 +137,23 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -135,7 +175,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -382,231 +425,248 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4">
-        <v>41244.0</v>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3">
-        <v>2012.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D5" s="3" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4">
-        <v>41246.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="D12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3">
-        <v>2012.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="D7" s="3" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="3">
-        <v>2012.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3">
-        <v>6.0</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="4">
-        <v>41246.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3">
-        <v>7.0</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4">
-        <v>41250.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="3">
-        <v>2012.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="4">
-        <v>41244.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="3">
-        <v>2012.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="4">
-        <v>41246.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4">
-        <v>41244.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>24</v>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C1:D1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Excel:   - Actualizo el archivo de DA segun lo que paso Pablo   - Creo LectoExcel.getValor() que se fija si es una celda numerica y la     trasnforma en String
</commit_message>
<xml_diff>
--- a/src/main/resources/ejemploDA.xlsx
+++ b/src/main/resources/ejemploDA.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
   <si>
     <t>Actividad</t>
   </si>
@@ -43,7 +43,7 @@
     <t>Mensual</t>
   </si>
   <si>
-    <t>12/2012</t>
+    <t>may-2022</t>
   </si>
   <si>
     <t>Diesel</t>
@@ -118,7 +118,22 @@
     <t>Logística de productos y residuos</t>
   </si>
   <si>
-    <t>??</t>
+    <t>Producto Transportado</t>
+  </si>
+  <si>
+    <t>Materia prima</t>
+  </si>
+  <si>
+    <t>Medio Transporte</t>
+  </si>
+  <si>
+    <t>Camion</t>
+  </si>
+  <si>
+    <t>Distancia Media</t>
+  </si>
+  <si>
+    <t>Peso Total</t>
   </si>
 </sst>
 </file>
@@ -185,7 +200,18 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -653,13 +679,64 @@
         <v>35</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="3">
+        <v>4500.0</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -669,6 +746,11 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E2"/>
   </mergeCells>
+  <conditionalFormatting sqref="C3:C15">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(C3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
huella de carbono calculado y agente sectorial creo que hecho
</commit_message>
<xml_diff>
--- a/src/main/resources/ejemploDA.xlsx
+++ b/src/main/resources/ejemploDA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>Actividad</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>052022</t>
+  </si>
+  <si>
+    <t>4500.33</t>
   </si>
 </sst>
 </file>
@@ -213,6 +216,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -220,8 +225,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,8 +454,8 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -463,30 +466,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
@@ -620,7 +623,7 @@
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -654,7 +657,7 @@
       <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -688,7 +691,7 @@
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -705,7 +708,7 @@
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -722,7 +725,7 @@
       <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -739,7 +742,7 @@
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -751,12 +754,12 @@
         <v>38</v>
       </c>
       <c r="C18" s="1">
-        <v>40</v>
+        <v>40.33</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -767,13 +770,13 @@
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="1">
-        <v>4500</v>
+      <c r="C19" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="4" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>